<commit_message>
Added more details to the sheetmetal spreadsheet.
</commit_message>
<xml_diff>
--- a/Sheetmetal/Quantity and Info Spreedsheet.xlsx
+++ b/Sheetmetal/Quantity and Info Spreedsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arjun\Desktop\Cad 2015\Sheetmetal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arjun\Desktop\Cad 2015\Nighthawk CAD\Sheetmetal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>Part Number/Name</t>
   </si>
@@ -44,130 +44,94 @@
     <t>Purpose</t>
   </si>
   <si>
-    <t>P_01</t>
-  </si>
-  <si>
     <t>Aluminum</t>
   </si>
   <si>
-    <t>Electrical Board</t>
-  </si>
-  <si>
-    <t>P_03</t>
-  </si>
-  <si>
-    <t>CRIO/D-Link/Other Mount</t>
-  </si>
-  <si>
-    <t>P_04</t>
-  </si>
-  <si>
-    <t>Shooter Housing Bottom</t>
-  </si>
-  <si>
-    <t>P_08</t>
-  </si>
-  <si>
-    <t>Sidecar Mounting/shelf</t>
-  </si>
-  <si>
-    <t>P_09</t>
-  </si>
-  <si>
-    <t>Battery Holder</t>
-  </si>
-  <si>
-    <t>P_15</t>
-  </si>
-  <si>
-    <t>Shooter housing Mount Hinge</t>
-  </si>
-  <si>
-    <t>P_19</t>
-  </si>
-  <si>
-    <t>Shooter Side Brace R</t>
-  </si>
-  <si>
-    <t>P_20</t>
-  </si>
-  <si>
-    <t>Shooter Side Brace L</t>
-  </si>
-  <si>
-    <t>P_21</t>
-  </si>
-  <si>
-    <t>shooter Bearing Mounts</t>
-  </si>
-  <si>
-    <t>P_22</t>
-  </si>
-  <si>
-    <t>Shooter Hinge Mounting</t>
-  </si>
-  <si>
-    <t>P_24</t>
-  </si>
-  <si>
-    <t>Shooter Gearbox Plates</t>
-  </si>
-  <si>
-    <t>P_25</t>
-  </si>
-  <si>
-    <t>Shooter Housing Top</t>
-  </si>
-  <si>
-    <t>P_26</t>
-  </si>
-  <si>
-    <t>Shooting Gearbox Mounting Piece</t>
-  </si>
-  <si>
-    <t>P_27</t>
-  </si>
-  <si>
-    <t>Shooter Housing Front</t>
-  </si>
-  <si>
-    <t>P_30</t>
-  </si>
-  <si>
-    <t>Thin Piece Shooter Disk</t>
-  </si>
-  <si>
-    <t>P_31</t>
-  </si>
-  <si>
-    <t>Shooter Disk Spacer</t>
-  </si>
-  <si>
-    <t>P_32</t>
-  </si>
-  <si>
-    <t>Shooter Disk Sprocket</t>
-  </si>
-  <si>
-    <t>P_34</t>
-  </si>
-  <si>
-    <t>Shooter Disk Main Piece</t>
-  </si>
-  <si>
-    <t>P_35</t>
-  </si>
-  <si>
-    <t>"Choo-Choo" Mechanism Arm Thick</t>
-  </si>
-  <si>
-    <t>P_36</t>
-  </si>
-  <si>
-    <t>"Choo-Choo" Mechanism Arm Thin</t>
-  </si>
-  <si>
-    <t>3/32''</t>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>P-1</t>
+  </si>
+  <si>
+    <t>P-2</t>
+  </si>
+  <si>
+    <t>P-3</t>
+  </si>
+  <si>
+    <t>P-4</t>
+  </si>
+  <si>
+    <t>P-5</t>
+  </si>
+  <si>
+    <t>P-6</t>
+  </si>
+  <si>
+    <t>P-7</t>
+  </si>
+  <si>
+    <t>P-8</t>
+  </si>
+  <si>
+    <t>P-9</t>
+  </si>
+  <si>
+    <t>P-10</t>
+  </si>
+  <si>
+    <t>P-11</t>
+  </si>
+  <si>
+    <t>P-12</t>
+  </si>
+  <si>
+    <t>P-13</t>
+  </si>
+  <si>
+    <t>P-14</t>
+  </si>
+  <si>
+    <t>P-15</t>
+  </si>
+  <si>
+    <t>P-16</t>
+  </si>
+  <si>
+    <t>P-17</t>
+  </si>
+  <si>
+    <t>P-18</t>
+  </si>
+  <si>
+    <t>P-19</t>
+  </si>
+  <si>
+    <t>P-20</t>
+  </si>
+  <si>
+    <t>Drive Module</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Front Gearbox</t>
+  </si>
+  <si>
+    <t>Battery Mount</t>
+  </si>
+  <si>
+    <t>Top of Elevator</t>
+  </si>
+  <si>
+    <t>Elevator Supports</t>
+  </si>
+  <si>
+    <t>Elevator Slides</t>
+  </si>
+  <si>
+    <t>Base Plate</t>
   </si>
 </sst>
 </file>
@@ -494,7 +458,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,18 +493,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -548,304 +512,276 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C19" s="2"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C20" s="2"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C21" s="2"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="F21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added more to the sheetmetal folder
</commit_message>
<xml_diff>
--- a/Sheetmetal/Quantity and Info Spreedsheet.xlsx
+++ b/Sheetmetal/Quantity and Info Spreedsheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>Part Number/Name</t>
   </si>
@@ -132,6 +132,27 @@
   </si>
   <si>
     <t>Base Plate</t>
+  </si>
+  <si>
+    <t>1/4''</t>
+  </si>
+  <si>
+    <t>Claw Plate</t>
+  </si>
+  <si>
+    <t>1/8''</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no </t>
+  </si>
+  <si>
+    <t>Claw Slide Plate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Claw Support </t>
+  </si>
+  <si>
+    <t>Claw Support Other Side</t>
   </si>
 </sst>
 </file>
@@ -458,7 +479,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,10 +727,16 @@
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="1"/>
+      <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -718,10 +745,16 @@
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="1"/>
+      <c r="C16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -730,10 +763,16 @@
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="1"/>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -742,10 +781,16 @@
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="1"/>
+      <c r="C18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">

</xml_diff>